<commit_message>
add resumo and xls
</commit_message>
<xml_diff>
--- a/experiment_1/notebooks/estrategias.xlsx
+++ b/experiment_1/notebooks/estrategias.xlsx
@@ -14,11 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Estratégia</t>
   </si>
   <si>
+    <t>Related</t>
+  </si>
+  <si>
+    <t>Visited</t>
+  </si>
+  <si>
+    <t>Final Selected</t>
+  </si>
+  <si>
     <t>Precision</t>
   </si>
   <si>
@@ -26,6 +35,15 @@
   </si>
   <si>
     <t>F-Measure</t>
+  </si>
+  <si>
+    <t>Final Precision</t>
+  </si>
+  <si>
+    <t>Final Recall</t>
+  </si>
+  <si>
+    <t>Final F-Measure</t>
   </si>
   <si>
     <t>E1</t>
@@ -404,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,124 +444,268 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>497</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>0.04426559356136821</v>
+      </c>
+      <c r="G2">
+        <v>0.4313725490196079</v>
+      </c>
+      <c r="H2">
+        <v>0.08029197080291971</v>
+      </c>
+      <c r="I2">
+        <v>0.03018108651911469</v>
+      </c>
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.05692599620493359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>1873</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>0.02722904431393487</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.05301455301455301</v>
+      </c>
+      <c r="I3">
+        <v>0.01601708489054992</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.03152916447714135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>1059</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>0.0339943342776204</v>
+      </c>
+      <c r="G4">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="H4">
+        <v>0.06486486486486487</v>
+      </c>
+      <c r="I4">
+        <v>0.02077431539187913</v>
+      </c>
+      <c r="J4">
+        <v>0.7333333333333333</v>
+      </c>
+      <c r="K4">
+        <v>0.04040404040404041</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>1174</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>0.03747870528109029</v>
+      </c>
+      <c r="G5">
+        <v>0.8627450980392157</v>
+      </c>
+      <c r="H5">
+        <v>0.07183673469387755</v>
+      </c>
+      <c r="I5">
+        <v>0.02129471890971039</v>
+      </c>
+      <c r="J5">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="K5">
+        <v>0.04152823920265781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>292</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>0.06506849315068493</v>
+      </c>
+      <c r="G6">
+        <v>0.3725490196078431</v>
+      </c>
+      <c r="H6">
+        <v>0.1107871720116618</v>
+      </c>
+      <c r="I6">
+        <v>0.04794520547945205</v>
+      </c>
+      <c r="J6">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="K6">
+        <v>0.08695652173913043</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>565</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>0.06194690265486726</v>
+      </c>
+      <c r="G7">
+        <v>0.6862745098039216</v>
+      </c>
+      <c r="H7">
+        <v>0.1136363636363636</v>
+      </c>
+      <c r="I7">
+        <v>0.03539823008849557</v>
+      </c>
+      <c r="J7">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K7">
+        <v>0.06722689075630252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>413</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>0.05811138014527845</v>
+      </c>
+      <c r="G8">
         <v>0.4705882352941176</v>
       </c>
-      <c r="D2">
-        <v>0.1568627450980392</v>
-      </c>
-      <c r="E2">
-        <v>0.2352941176470588</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>0.03069236259814418</v>
-      </c>
-      <c r="D3">
-        <v>0.8431372549019608</v>
-      </c>
-      <c r="E3">
-        <v>0.05922865013774105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>0.04298356510745891</v>
-      </c>
-      <c r="D4">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="E4">
-        <v>0.08076009501187648</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>0.04627539503386004</v>
-      </c>
-      <c r="D5">
-        <v>0.803921568627451</v>
-      </c>
-      <c r="E5">
-        <v>0.08751334044823907</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>0.06551724137931035</v>
-      </c>
-      <c r="D6">
-        <v>0.3725490196078431</v>
-      </c>
-      <c r="E6">
-        <v>0.1114369501466276</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>0.07888631090487239</v>
-      </c>
-      <c r="D7">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="E7">
-        <v>0.1410788381742738</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>0.0583941605839416</v>
-      </c>
-      <c r="D8">
-        <v>0.4705882352941176</v>
-      </c>
-      <c r="E8">
-        <v>0.1038961038961039</v>
+      <c r="H8">
+        <v>0.103448275862069</v>
+      </c>
+      <c r="I8">
+        <v>0.03631961259079903</v>
+      </c>
+      <c r="J8">
+        <v>0.5</v>
+      </c>
+      <c r="K8">
+        <v>0.06772009029345372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resumo atualizado do experimento 1
</commit_message>
<xml_diff>
--- a/experiment_1/notebooks/estrategias.xlsx
+++ b/experiment_1/notebooks/estrategias.xlsx
@@ -471,31 +471,31 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D2">
-        <v>497</v>
+        <v>1873</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F2">
-        <v>0.04426559356136821</v>
+        <v>0.03</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.08477842003853565</v>
+        <v>0.05</v>
       </c>
       <c r="I2">
-        <v>0.03018108651911469</v>
+        <v>0.02</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>0.05692599620493359</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -515,22 +515,22 @@
         <v>30</v>
       </c>
       <c r="F3">
-        <v>0.02722904431393487</v>
+        <v>0.03</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.05301455301455301</v>
+        <v>0.05</v>
       </c>
       <c r="I3">
-        <v>0.01601708489054992</v>
+        <v>0.02</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0.03152916447714135</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -550,22 +550,22 @@
         <v>22</v>
       </c>
       <c r="F4">
-        <v>0.0339943342776204</v>
+        <v>0.03</v>
       </c>
       <c r="G4">
-        <v>0.7058823529411765</v>
+        <v>0.71</v>
       </c>
       <c r="H4">
-        <v>0.06486486486486487</v>
+        <v>0.06</v>
       </c>
       <c r="I4">
-        <v>0.02077431539187913</v>
+        <v>0.02</v>
       </c>
       <c r="J4">
-        <v>0.7333333333333333</v>
+        <v>0.73</v>
       </c>
       <c r="K4">
-        <v>0.04040404040404041</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -585,22 +585,22 @@
         <v>25</v>
       </c>
       <c r="F5">
-        <v>0.03747870528109029</v>
+        <v>0.04</v>
       </c>
       <c r="G5">
-        <v>0.8627450980392157</v>
+        <v>0.86</v>
       </c>
       <c r="H5">
-        <v>0.07183673469387755</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I5">
-        <v>0.02129471890971039</v>
+        <v>0.02</v>
       </c>
       <c r="J5">
-        <v>0.8333333333333334</v>
+        <v>0.83</v>
       </c>
       <c r="K5">
-        <v>0.04152823920265781</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -620,22 +620,22 @@
         <v>14</v>
       </c>
       <c r="F6">
-        <v>0.06506849315068493</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G6">
-        <v>0.3725490196078431</v>
+        <v>0.37</v>
       </c>
       <c r="H6">
-        <v>0.1107871720116618</v>
+        <v>0.11</v>
       </c>
       <c r="I6">
-        <v>0.04794520547945205</v>
+        <v>0.05</v>
       </c>
       <c r="J6">
-        <v>0.4666666666666667</v>
+        <v>0.47</v>
       </c>
       <c r="K6">
-        <v>0.08695652173913043</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -655,22 +655,22 @@
         <v>20</v>
       </c>
       <c r="F7">
-        <v>0.06194690265486726</v>
+        <v>0.06</v>
       </c>
       <c r="G7">
-        <v>0.6862745098039216</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H7">
-        <v>0.1136363636363636</v>
+        <v>0.11</v>
       </c>
       <c r="I7">
-        <v>0.03539823008849557</v>
+        <v>0.04</v>
       </c>
       <c r="J7">
-        <v>0.6666666666666666</v>
+        <v>0.67</v>
       </c>
       <c r="K7">
-        <v>0.06722689075630252</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -690,22 +690,22 @@
         <v>15</v>
       </c>
       <c r="F8">
-        <v>0.05811138014527845</v>
+        <v>0.06</v>
       </c>
       <c r="G8">
-        <v>0.4705882352941176</v>
+        <v>0.47</v>
       </c>
       <c r="H8">
-        <v>0.103448275862069</v>
+        <v>0.1</v>
       </c>
       <c r="I8">
-        <v>0.03631961259079903</v>
+        <v>0.04</v>
       </c>
       <c r="J8">
         <v>0.5</v>
       </c>
       <c r="K8">
-        <v>0.06772009029345372</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes no estrategia - grafo e citacao
</commit_message>
<xml_diff>
--- a/experiment_1/notebooks/estrategias.xlsx
+++ b/experiment_1/notebooks/estrategias.xlsx
@@ -471,31 +471,31 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D2">
-        <v>43</v>
+        <v>497</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F2">
-        <v>0.1395348837209302</v>
+        <v>0.04</v>
       </c>
       <c r="G2">
-        <v>0.1176470588235294</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>0.1276595744680851</v>
+        <v>0.08</v>
       </c>
       <c r="I2">
-        <v>0.09302325581395349</v>
+        <v>0.03</v>
       </c>
       <c r="J2">
-        <v>0.1333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="K2">
-        <v>0.1095890410958904</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -515,22 +515,22 @@
         <v>30</v>
       </c>
       <c r="F3">
-        <v>0.02722904431393487</v>
+        <v>0.03</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.05301455301455301</v>
+        <v>0.05</v>
       </c>
       <c r="I3">
-        <v>0.01601708489054992</v>
+        <v>0.02</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0.03152916447714135</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -550,22 +550,22 @@
         <v>22</v>
       </c>
       <c r="F4">
-        <v>0.0339943342776204</v>
+        <v>0.03</v>
       </c>
       <c r="G4">
-        <v>0.7058823529411765</v>
+        <v>0.71</v>
       </c>
       <c r="H4">
-        <v>0.06486486486486487</v>
+        <v>0.06</v>
       </c>
       <c r="I4">
-        <v>0.02077431539187913</v>
+        <v>0.02</v>
       </c>
       <c r="J4">
-        <v>0.7333333333333333</v>
+        <v>0.73</v>
       </c>
       <c r="K4">
-        <v>0.04040404040404041</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -585,22 +585,22 @@
         <v>25</v>
       </c>
       <c r="F5">
-        <v>0.03747870528109029</v>
+        <v>0.04</v>
       </c>
       <c r="G5">
-        <v>0.8627450980392157</v>
+        <v>0.86</v>
       </c>
       <c r="H5">
-        <v>0.07183673469387755</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I5">
-        <v>0.02129471890971039</v>
+        <v>0.02</v>
       </c>
       <c r="J5">
-        <v>0.8333333333333334</v>
+        <v>0.83</v>
       </c>
       <c r="K5">
-        <v>0.04152823920265781</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -620,22 +620,22 @@
         <v>14</v>
       </c>
       <c r="F6">
-        <v>0.06506849315068493</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G6">
-        <v>0.3725490196078431</v>
+        <v>0.37</v>
       </c>
       <c r="H6">
-        <v>0.1107871720116618</v>
+        <v>0.11</v>
       </c>
       <c r="I6">
-        <v>0.04794520547945205</v>
+        <v>0.05</v>
       </c>
       <c r="J6">
-        <v>0.4666666666666667</v>
+        <v>0.47</v>
       </c>
       <c r="K6">
-        <v>0.08695652173913043</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -655,22 +655,22 @@
         <v>20</v>
       </c>
       <c r="F7">
-        <v>0.06194690265486726</v>
+        <v>0.06</v>
       </c>
       <c r="G7">
-        <v>0.6862745098039216</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H7">
-        <v>0.1136363636363636</v>
+        <v>0.11</v>
       </c>
       <c r="I7">
-        <v>0.03539823008849557</v>
+        <v>0.04</v>
       </c>
       <c r="J7">
-        <v>0.6666666666666666</v>
+        <v>0.67</v>
       </c>
       <c r="K7">
-        <v>0.06722689075630252</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -690,22 +690,22 @@
         <v>15</v>
       </c>
       <c r="F8">
-        <v>0.05811138014527845</v>
+        <v>0.06</v>
       </c>
       <c r="G8">
-        <v>0.4705882352941176</v>
+        <v>0.47</v>
       </c>
       <c r="H8">
-        <v>0.103448275862069</v>
+        <v>0.1</v>
       </c>
       <c r="I8">
-        <v>0.03631961259079903</v>
+        <v>0.04</v>
       </c>
       <c r="J8">
         <v>0.5</v>
       </c>
       <c r="K8">
-        <v>0.06772009029345372</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>